<commit_message>
Updated Acceptance Test Plan
</commit_message>
<xml_diff>
--- a/etc/Acceptance Test Plan.xlsx
+++ b/etc/Acceptance Test Plan.xlsx
@@ -12,7 +12,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="112" uniqueCount="59">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="167" uniqueCount="93">
   <si>
     <t>Instructions</t>
   </si>
@@ -194,6 +194,108 @@
   </si>
   <si>
     <t>Given I'm on the cart page when I click a product's remove from cart button then the product gets removed from my cart.</t>
+  </si>
+  <si>
+    <t>As a Developer, I want to checkout a Buyer’s shopping cart, so that they can possibly unlock new products and update the inventory’s quantity of products.</t>
+  </si>
+  <si>
+    <t>Given that two products in a user's shopping cart combine when a request is made to POST /users/checkout, then the user should unlock the new product, have their shopping cart cleared, decrease the quantity of the two initial products, and receive a 200 (OK) with the unlocked product.</t>
+  </si>
+  <si>
+    <t>N/A</t>
+  </si>
+  <si>
+    <t>Given that two products in a user's shopping cart do not combine when a request is made to POST /users/checkout, then the user should have their shopping cart cleared, decrease the quantity of the two initial products, and receive a 404 (NOT FOUND).</t>
+  </si>
+  <si>
+    <t>Given that less than two products are in a user's shopping cart when a request is made to POST /users/checkout, then the user should receive a 400 (Bad Request).</t>
+  </si>
+  <si>
+    <t>Given that two products in a user's shopping cart do not combine when a request is made to POST /users/checkout and at least one product is sold out, then the user should receive 400 (Bad Request).</t>
+  </si>
+  <si>
+    <t>As a Buyer, I want to be able to sort products on the products page, so that I can find the product I want to buy.</t>
+  </si>
+  <si>
+    <t>Given I'm on the products page when I click the sort by price from high to low button then the products get sorted by price from high to low.</t>
+  </si>
+  <si>
+    <t>Given I'm on the products page when I click the sort by price from low to high button then the products get sorted by price from low to high.</t>
+  </si>
+  <si>
+    <t>Given I'm on the products page when I click the sort alphabetically button then the products get sorted alphabetically.</t>
+  </si>
+  <si>
+    <t>As a Buyer, I want to filter by type, unlocked or locked, and other useful attributes, so that I can easily find products on the store.</t>
+  </si>
+  <si>
+    <t>Given I have opened the filter menu when I select a specific type to filter by then I should see only products matching the type.</t>
+  </si>
+  <si>
+    <t>Given I am on the catalog page when I enable the unlocked products filter then I expect only to see products I have unlocked.</t>
+  </si>
+  <si>
+    <t>Given I am on the catalog page when I enable the locked products filter then I expect only to see products I have locked.</t>
+  </si>
+  <si>
+    <t>As a Buyer, I want my password to meet minimum strength requirements (e.g., 8 characters, 1 capital, 1 symbol, 1 number), so that I can maintain a secure account.</t>
+  </si>
+  <si>
+    <t>Given that I try to create an account password on the register page when I enter a password that meets the requirements of (8 characters, 1 capital, 1 symbol, and 1 number) then the password will be accepted and assigned to the user.</t>
+  </si>
+  <si>
+    <t>Given that I try to create an account password on the register page when I enter a password that does not contain (8 characters, 1 capital, 1 symbol, and 1 number) then the password will not be accepted, and the user will have to enter a new password.</t>
+  </si>
+  <si>
+    <t>As an Owner or Buyer, I want my password to be stored in hashed form on file, so that my account is less vulnerable to being compromised in case of a leak.</t>
+  </si>
+  <si>
+    <t>Given a plaintext password is passed when a POST /users request is received then the password field should be modified to its hashed version instead of plaintext.</t>
+  </si>
+  <si>
+    <t>Given a plaintext password is passed when a POST /users/auth request is received and the password matches the hashed version then it should respond with 200 (OK) and the stored user (without their password).</t>
+  </si>
+  <si>
+    <t>Given a plaintext password is passed when a POST /users/auth request is received and the password does not match the hased version then it should respond with 401 (Unauthorized).</t>
+  </si>
+  <si>
+    <t>As a Developer, I want a global stylesheet made for the site, so that I can extend its styling to specific pages later on to create a cohesive UI experience.</t>
+  </si>
+  <si>
+    <t>Given that I view any page on the site when that page has commonly used elements then I expect them to be styled consistently.</t>
+  </si>
+  <si>
+    <t>As an Owner or Buyer, I want the login/registering page to be well-styled, so that the experience is user-friendly and aesthetically pleasing.</t>
+  </si>
+  <si>
+    <t>Given I am on the login and registering page when I am viewing the pages then the elements on the page should be styled well and user-friendly.</t>
+  </si>
+  <si>
+    <t>As a Buyer of the site, I want the experience of browsing products in the catalog to be user-friendly and aesthetically pleasing, so that the site is pleasant to use.</t>
+  </si>
+  <si>
+    <t>Given I am on the catalog page when I am browsing products then I should be able to efficiently and pleasingly see all products.</t>
+  </si>
+  <si>
+    <t>As a Buyer, I want the cart page to be well-styled and easy to use so that the shopping cart experience goes smoothly.</t>
+  </si>
+  <si>
+    <t>Given I am on the cart page when I am viewing my cart then I can efficiently add and remove items from my cart on a well-styled page.</t>
+  </si>
+  <si>
+    <t>As an Owner, I want to be able to efficiently navigate and use the admin features on well-styled pages, so that using the site is a user-friendly experience.</t>
+  </si>
+  <si>
+    <t>Given I am on the admin page when I use the admin features then they are well-styled and easy to use.</t>
+  </si>
+  <si>
+    <t>As a Developer, I want to be able to have a predefined JSON mapping of products that combine, so that Buyers can unlock products based on their cart later.</t>
+  </si>
+  <si>
+    <t>Given I look up the combination of two products when those two products combine then I expect the result to be stored in crafting.json.</t>
+  </si>
+  <si>
+    <t>Given I look up the combination of two products when those two products do not combine then I expect the result to not be present in crafting.json.</t>
   </si>
 </sst>
 </file>
@@ -4691,10 +4793,16 @@
       <c r="Z30" s="12"/>
     </row>
     <row r="31" ht="15.75" customHeight="1">
-      <c r="A31" s="2"/>
-      <c r="B31" s="2"/>
+      <c r="A31" s="9" t="s">
+        <v>59</v>
+      </c>
+      <c r="B31" s="9" t="s">
+        <v>60</v>
+      </c>
       <c r="C31" s="11"/>
-      <c r="D31" s="2"/>
+      <c r="D31" s="9" t="s">
+        <v>61</v>
+      </c>
       <c r="E31" s="11"/>
       <c r="F31" s="2"/>
       <c r="G31" s="12"/>
@@ -4720,9 +4828,13 @@
     </row>
     <row r="32" ht="15.75" customHeight="1">
       <c r="A32" s="2"/>
-      <c r="B32" s="2"/>
+      <c r="B32" s="9" t="s">
+        <v>62</v>
+      </c>
       <c r="C32" s="11"/>
-      <c r="D32" s="2"/>
+      <c r="D32" s="9" t="s">
+        <v>61</v>
+      </c>
       <c r="E32" s="11"/>
       <c r="F32" s="2"/>
       <c r="G32" s="12"/>
@@ -4748,9 +4860,13 @@
     </row>
     <row r="33" ht="15.75" customHeight="1">
       <c r="A33" s="2"/>
-      <c r="B33" s="2"/>
+      <c r="B33" s="9" t="s">
+        <v>63</v>
+      </c>
       <c r="C33" s="11"/>
-      <c r="D33" s="2"/>
+      <c r="D33" s="9" t="s">
+        <v>61</v>
+      </c>
       <c r="E33" s="11"/>
       <c r="F33" s="2"/>
       <c r="G33" s="12"/>
@@ -4775,10 +4891,14 @@
       <c r="Z33" s="12"/>
     </row>
     <row r="34" ht="15.75" customHeight="1">
-      <c r="A34" s="2"/>
-      <c r="B34" s="2"/>
+      <c r="A34" s="16"/>
+      <c r="B34" s="17" t="s">
+        <v>64</v>
+      </c>
       <c r="C34" s="11"/>
-      <c r="D34" s="2"/>
+      <c r="D34" s="9" t="s">
+        <v>61</v>
+      </c>
       <c r="E34" s="11"/>
       <c r="F34" s="2"/>
       <c r="G34" s="12"/>
@@ -4803,10 +4923,16 @@
       <c r="Z34" s="12"/>
     </row>
     <row r="35" ht="15.75" customHeight="1">
-      <c r="A35" s="2"/>
-      <c r="B35" s="2"/>
+      <c r="A35" s="9" t="s">
+        <v>65</v>
+      </c>
+      <c r="B35" s="9" t="s">
+        <v>66</v>
+      </c>
       <c r="C35" s="11"/>
-      <c r="D35" s="2"/>
+      <c r="D35" s="9" t="s">
+        <v>61</v>
+      </c>
       <c r="E35" s="11"/>
       <c r="F35" s="2"/>
       <c r="G35" s="12"/>
@@ -4832,9 +4958,13 @@
     </row>
     <row r="36" ht="15.75" customHeight="1">
       <c r="A36" s="2"/>
-      <c r="B36" s="2"/>
+      <c r="B36" s="9" t="s">
+        <v>67</v>
+      </c>
       <c r="C36" s="11"/>
-      <c r="D36" s="2"/>
+      <c r="D36" s="9" t="s">
+        <v>61</v>
+      </c>
       <c r="E36" s="11"/>
       <c r="F36" s="2"/>
       <c r="G36" s="12"/>
@@ -4859,10 +4989,14 @@
       <c r="Z36" s="12"/>
     </row>
     <row r="37" ht="15.75" customHeight="1">
-      <c r="A37" s="2"/>
-      <c r="B37" s="2"/>
+      <c r="A37" s="16"/>
+      <c r="B37" s="17" t="s">
+        <v>68</v>
+      </c>
       <c r="C37" s="11"/>
-      <c r="D37" s="2"/>
+      <c r="D37" s="9" t="s">
+        <v>61</v>
+      </c>
       <c r="E37" s="11"/>
       <c r="F37" s="2"/>
       <c r="G37" s="12"/>
@@ -4887,10 +5021,16 @@
       <c r="Z37" s="12"/>
     </row>
     <row r="38" ht="15.75" customHeight="1">
-      <c r="A38" s="2"/>
-      <c r="B38" s="2"/>
+      <c r="A38" s="9" t="s">
+        <v>69</v>
+      </c>
+      <c r="B38" s="9" t="s">
+        <v>70</v>
+      </c>
       <c r="C38" s="11"/>
-      <c r="D38" s="2"/>
+      <c r="D38" s="9" t="s">
+        <v>61</v>
+      </c>
       <c r="E38" s="11"/>
       <c r="F38" s="2"/>
       <c r="G38" s="12"/>
@@ -4916,9 +5056,13 @@
     </row>
     <row r="39" ht="15.75" customHeight="1">
       <c r="A39" s="2"/>
-      <c r="B39" s="2"/>
+      <c r="B39" s="9" t="s">
+        <v>71</v>
+      </c>
       <c r="C39" s="11"/>
-      <c r="D39" s="2"/>
+      <c r="D39" s="9" t="s">
+        <v>61</v>
+      </c>
       <c r="E39" s="11"/>
       <c r="F39" s="2"/>
       <c r="G39" s="12"/>
@@ -4943,10 +5087,14 @@
       <c r="Z39" s="12"/>
     </row>
     <row r="40" ht="15.75" customHeight="1">
-      <c r="A40" s="2"/>
-      <c r="B40" s="2"/>
+      <c r="A40" s="16"/>
+      <c r="B40" s="17" t="s">
+        <v>72</v>
+      </c>
       <c r="C40" s="11"/>
-      <c r="D40" s="2"/>
+      <c r="D40" s="9" t="s">
+        <v>61</v>
+      </c>
       <c r="E40" s="11"/>
       <c r="F40" s="2"/>
       <c r="G40" s="12"/>
@@ -4971,10 +5119,16 @@
       <c r="Z40" s="12"/>
     </row>
     <row r="41" ht="15.75" customHeight="1">
-      <c r="A41" s="2"/>
-      <c r="B41" s="2"/>
+      <c r="A41" s="9" t="s">
+        <v>73</v>
+      </c>
+      <c r="B41" s="9" t="s">
+        <v>74</v>
+      </c>
       <c r="C41" s="11"/>
-      <c r="D41" s="2"/>
+      <c r="D41" s="9" t="s">
+        <v>61</v>
+      </c>
       <c r="E41" s="11"/>
       <c r="F41" s="2"/>
       <c r="G41" s="12"/>
@@ -4999,10 +5153,14 @@
       <c r="Z41" s="12"/>
     </row>
     <row r="42" ht="15.75" customHeight="1">
-      <c r="A42" s="2"/>
-      <c r="B42" s="2"/>
+      <c r="A42" s="16"/>
+      <c r="B42" s="17" t="s">
+        <v>75</v>
+      </c>
       <c r="C42" s="11"/>
-      <c r="D42" s="2"/>
+      <c r="D42" s="9" t="s">
+        <v>61</v>
+      </c>
       <c r="E42" s="11"/>
       <c r="F42" s="2"/>
       <c r="G42" s="12"/>
@@ -5027,10 +5185,16 @@
       <c r="Z42" s="12"/>
     </row>
     <row r="43" ht="15.75" customHeight="1">
-      <c r="A43" s="2"/>
-      <c r="B43" s="2"/>
+      <c r="A43" s="9" t="s">
+        <v>76</v>
+      </c>
+      <c r="B43" s="9" t="s">
+        <v>77</v>
+      </c>
       <c r="C43" s="11"/>
-      <c r="D43" s="2"/>
+      <c r="D43" s="9" t="s">
+        <v>61</v>
+      </c>
       <c r="E43" s="11"/>
       <c r="F43" s="2"/>
       <c r="G43" s="12"/>
@@ -5056,9 +5220,13 @@
     </row>
     <row r="44" ht="15.75" customHeight="1">
       <c r="A44" s="2"/>
-      <c r="B44" s="2"/>
+      <c r="B44" s="9" t="s">
+        <v>78</v>
+      </c>
       <c r="C44" s="11"/>
-      <c r="D44" s="2"/>
+      <c r="D44" s="9" t="s">
+        <v>61</v>
+      </c>
       <c r="E44" s="11"/>
       <c r="F44" s="2"/>
       <c r="G44" s="12"/>
@@ -5083,10 +5251,14 @@
       <c r="Z44" s="12"/>
     </row>
     <row r="45" ht="15.75" customHeight="1">
-      <c r="A45" s="2"/>
-      <c r="B45" s="2"/>
+      <c r="A45" s="16"/>
+      <c r="B45" s="17" t="s">
+        <v>79</v>
+      </c>
       <c r="C45" s="11"/>
-      <c r="D45" s="2"/>
+      <c r="D45" s="9" t="s">
+        <v>61</v>
+      </c>
       <c r="E45" s="11"/>
       <c r="F45" s="2"/>
       <c r="G45" s="12"/>
@@ -5111,10 +5283,16 @@
       <c r="Z45" s="12"/>
     </row>
     <row r="46" ht="15.75" customHeight="1">
-      <c r="A46" s="2"/>
-      <c r="B46" s="2"/>
+      <c r="A46" s="17" t="s">
+        <v>80</v>
+      </c>
+      <c r="B46" s="17" t="s">
+        <v>81</v>
+      </c>
       <c r="C46" s="11"/>
-      <c r="D46" s="2"/>
+      <c r="D46" s="9" t="s">
+        <v>61</v>
+      </c>
       <c r="E46" s="11"/>
       <c r="F46" s="2"/>
       <c r="G46" s="12"/>
@@ -5139,10 +5317,16 @@
       <c r="Z46" s="12"/>
     </row>
     <row r="47" ht="15.75" customHeight="1">
-      <c r="A47" s="2"/>
-      <c r="B47" s="2"/>
+      <c r="A47" s="17" t="s">
+        <v>82</v>
+      </c>
+      <c r="B47" s="17" t="s">
+        <v>83</v>
+      </c>
       <c r="C47" s="11"/>
-      <c r="D47" s="2"/>
+      <c r="D47" s="9" t="s">
+        <v>61</v>
+      </c>
       <c r="E47" s="11"/>
       <c r="F47" s="2"/>
       <c r="G47" s="12"/>
@@ -5167,10 +5351,16 @@
       <c r="Z47" s="12"/>
     </row>
     <row r="48" ht="15.75" customHeight="1">
-      <c r="A48" s="2"/>
-      <c r="B48" s="2"/>
+      <c r="A48" s="17" t="s">
+        <v>84</v>
+      </c>
+      <c r="B48" s="17" t="s">
+        <v>85</v>
+      </c>
       <c r="C48" s="11"/>
-      <c r="D48" s="2"/>
+      <c r="D48" s="9" t="s">
+        <v>61</v>
+      </c>
       <c r="E48" s="11"/>
       <c r="F48" s="2"/>
       <c r="G48" s="12"/>
@@ -5195,10 +5385,16 @@
       <c r="Z48" s="12"/>
     </row>
     <row r="49" ht="15.75" customHeight="1">
-      <c r="A49" s="2"/>
-      <c r="B49" s="2"/>
+      <c r="A49" s="17" t="s">
+        <v>86</v>
+      </c>
+      <c r="B49" s="17" t="s">
+        <v>87</v>
+      </c>
       <c r="C49" s="11"/>
-      <c r="D49" s="2"/>
+      <c r="D49" s="9" t="s">
+        <v>61</v>
+      </c>
       <c r="E49" s="11"/>
       <c r="F49" s="2"/>
       <c r="G49" s="12"/>
@@ -5223,10 +5419,16 @@
       <c r="Z49" s="12"/>
     </row>
     <row r="50" ht="15.75" customHeight="1">
-      <c r="A50" s="2"/>
-      <c r="B50" s="2"/>
+      <c r="A50" s="17" t="s">
+        <v>88</v>
+      </c>
+      <c r="B50" s="17" t="s">
+        <v>89</v>
+      </c>
       <c r="C50" s="11"/>
-      <c r="D50" s="2"/>
+      <c r="D50" s="9" t="s">
+        <v>61</v>
+      </c>
       <c r="E50" s="11"/>
       <c r="F50" s="2"/>
       <c r="G50" s="12"/>
@@ -5251,10 +5453,16 @@
       <c r="Z50" s="12"/>
     </row>
     <row r="51" ht="15.75" customHeight="1">
-      <c r="A51" s="2"/>
-      <c r="B51" s="2"/>
+      <c r="A51" s="9" t="s">
+        <v>90</v>
+      </c>
+      <c r="B51" s="9" t="s">
+        <v>91</v>
+      </c>
       <c r="C51" s="11"/>
-      <c r="D51" s="2"/>
+      <c r="D51" s="9" t="s">
+        <v>61</v>
+      </c>
       <c r="E51" s="11"/>
       <c r="F51" s="2"/>
       <c r="G51" s="12"/>
@@ -5279,10 +5487,14 @@
       <c r="Z51" s="12"/>
     </row>
     <row r="52" ht="15.75" customHeight="1">
-      <c r="A52" s="2"/>
-      <c r="B52" s="2"/>
+      <c r="A52" s="16"/>
+      <c r="B52" s="17" t="s">
+        <v>92</v>
+      </c>
       <c r="C52" s="11"/>
-      <c r="D52" s="2"/>
+      <c r="D52" s="9" t="s">
+        <v>61</v>
+      </c>
       <c r="E52" s="11"/>
       <c r="F52" s="2"/>
       <c r="G52" s="12"/>
@@ -5310,7 +5522,7 @@
       <c r="A53" s="2"/>
       <c r="B53" s="2"/>
       <c r="C53" s="11"/>
-      <c r="D53" s="2"/>
+      <c r="D53" s="9"/>
       <c r="E53" s="11"/>
       <c r="F53" s="2"/>
       <c r="G53" s="12"/>

</xml_diff>